<commit_message>
Changes regarding Alex & Ansgar
</commit_message>
<xml_diff>
--- a/TableData/Table7.xlsx
+++ b/TableData/Table7.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabler Arbeitsplatz\Documents\GitHub\ChristophKiesl.github.io\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Master Uni Ulm\2. Semester\Project Economic Data Science\ChristophKiesl.github.io\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8C7BEB-3B1B-4F76-A25A-3D512ECD1233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="15495"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Company_Name</t>
   </si>
@@ -56,39 +48,59 @@
     <t>Data Storage Corp</t>
   </si>
   <si>
-    <t xml:space="preserve">	AGILYSYS INC</t>
-  </si>
-  <si>
     <t>Kosmos Energy Ltd.</t>
   </si>
   <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Relevance</t>
+    <t>Accession ID</t>
+  </si>
+  <si>
+    <t>0000897101-17-000402</t>
+  </si>
+  <si>
+    <t>0001615774-19-005785</t>
+  </si>
+  <si>
+    <t>0001326380-18-000033</t>
   </si>
   <si>
     <t>FOCUS UNIVERSAL INC.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001683168-21-001026</t>
   </si>
   <si>
     <t>BIG LOTS INC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000768835-18-000030</t>
   </si>
   <si>
     <t>WEX Inc.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coherence</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001309108-23-000022</t>
+  </si>
+  <si>
+    <t>0000900075-23-000034</t>
+  </si>
+  <si>
+    <t>AGILYSYS INC</t>
+  </si>
+  <si>
+    <t>0001731122-20-000381</t>
+  </si>
+  <si>
+    <t>0000078749-17-000021</t>
+  </si>
+  <si>
+    <t>0001509991-21-000031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,186 +483,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.875" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2016</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>9.5</v>
-      </c>
-      <c r="E2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="C6">
         <v>2018</v>
       </c>
-      <c r="C3">
-        <v>9.5</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2018</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>2020</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>2018</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>2022</v>
       </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>2023</v>
       </c>
-      <c r="C8">
-        <v>8.5</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>2019</v>
       </c>
-      <c r="C9">
-        <v>8.5</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
+      <c r="C11">
         <v>2020</v>
       </c>
     </row>

</xml_diff>